<commit_message>
add captions in run file
</commit_message>
<xml_diff>
--- a/data/cases_data.xlsx
+++ b/data/cases_data.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20145" windowHeight="7770" activeTab="3"/>
+    <workbookView windowWidth="20145" windowHeight="7770" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="register" sheetId="2" r:id="rId2"/>
     <sheet name="recharge" sheetId="3" r:id="rId3"/>
     <sheet name="withdraw" sheetId="4" r:id="rId4"/>
+    <sheet name="add" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126">
   <si>
     <t>case_id</t>
   </si>
@@ -392,6 +393,9 @@
   </si>
   <si>
     <t>{ "code": 1002,"msg": "余额不足"}</t>
+  </si>
+  <si>
+    <t>添加成功</t>
   </si>
 </sst>
 </file>
@@ -399,10 +403,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -443,8 +447,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -459,15 +478,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -481,6 +499,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -488,32 +514,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -543,15 +545,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -578,13 +582,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,13 +654,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,145 +750,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -800,6 +804,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -816,15 +844,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -834,17 +853,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -863,21 +882,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -886,10 +890,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="7">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
@@ -898,16 +902,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
@@ -919,112 +923,112 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1628,7 +1632,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -2159,7 +2163,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -2441,8 +2445,8 @@
   <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -2606,4 +2610,57 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>